<commit_message>
Section 25 : fix section 25
</commit_message>
<xml_diff>
--- a/TN_Core_Web_App/wwwroot/templates/ProductImportTemplate.xlsx
+++ b/TN_Core_Web_App/wwwroot/templates/ProductImportTemplate.xlsx
@@ -2,19 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoct\Documents\Visual Studio 2017\Projects\TeduCore\TeduCore.WebApp\wwwroot\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,10 +21,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Original Price</t>
   </si>
   <si>
     <t>Price</t>
@@ -38,9 +36,6 @@
     <t>Promotion Price</t>
   </si>
   <si>
-    <t>Original Price</t>
-  </si>
-  <si>
     <t>Content</t>
   </si>
   <si>
@@ -53,16 +48,16 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Home Flag</t>
+  </si>
+  <si>
     <t>Hot Flag</t>
-  </si>
-  <si>
-    <t>Home Flag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,9 +172,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -212,9 +207,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -397,39 +392,39 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -444,10 +439,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>